<commit_message>
Ajout fonction api durée trajet
</commit_message>
<xml_diff>
--- a/Distances.xlsx
+++ b/Distances.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aellul\OneDrive - De Vinci\Documents\CoursESILV2022\Langage C# Initiaux\Problème\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99e27d525adb6305/ESILV/9. Langage C^N/Projet TransConnect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{677840F3-7433-4216-806D-3FEF656CC6F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{18D4C35F-A7A1-448A-A65C-CA5C2DC2D27E}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{677840F3-7433-4216-806D-3FEF656CC6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED328875-888B-47DF-8F5E-A508FDB9AC70}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8304" xr2:uid="{B8482291-9671-4883-824D-7A869219A0E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B8482291-9671-4883-824D-7A869219A0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Coordinates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Paris</t>
   </si>
@@ -123,19 +124,112 @@
   </si>
   <si>
     <t>1h35</t>
+  </si>
+  <si>
+    <t>2.333333</t>
+  </si>
+  <si>
+    <t>48.866667</t>
+  </si>
+  <si>
+    <t>-0.5593</t>
+  </si>
+  <si>
+    <t>47.4698</t>
+  </si>
+  <si>
+    <t>-1.150000</t>
+  </si>
+  <si>
+    <t>46.166667</t>
+  </si>
+  <si>
+    <t>44.833328 </t>
+  </si>
+  <si>
+    <t>-0.56667</t>
+  </si>
+  <si>
+    <t>-1.56667</t>
+  </si>
+  <si>
+    <t>43.48333</t>
+  </si>
+  <si>
+    <t>-0.366667</t>
+  </si>
+  <si>
+    <t>43.300000</t>
+  </si>
+  <si>
+    <t>1.433333</t>
+  </si>
+  <si>
+    <t>43.600000</t>
+  </si>
+  <si>
+    <t>3.862038</t>
+  </si>
+  <si>
+    <t>43.62505 </t>
+  </si>
+  <si>
+    <t>4.35</t>
+  </si>
+  <si>
+    <t>43.833328 </t>
+  </si>
+  <si>
+    <t>5.400000</t>
+  </si>
+  <si>
+    <t>7.424450755119324</t>
+  </si>
+  <si>
+    <t>43.738347784533</t>
+  </si>
+  <si>
+    <t>43.116669 </t>
+  </si>
+  <si>
+    <t>5.93333</t>
+  </si>
+  <si>
+    <t>4.850000</t>
+  </si>
+  <si>
+    <t>45.750000</t>
+  </si>
+  <si>
+    <t>4.81667</t>
+  </si>
+  <si>
+    <t>43.950001 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,8 +252,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -178,9 +274,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +314,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,7 +420,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,7 +562,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,13 +572,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F09E20F-1FB4-40EC-8AAA-24ACC53A1548}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -524,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -538,7 +634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -552,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -566,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -580,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -594,7 +690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -608,7 +704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -622,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -636,7 +732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -650,7 +746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -664,7 +760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -676,6 +772,179 @@
       </c>
       <c r="D14" t="s">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2845E1-D3FA-4206-9B0D-A06BC816AA90}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -684,21 +953,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -934,6 +1203,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E242C474-6AB9-443D-B939-8B932E7DF18F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7820E698-9C61-42D5-96C3-D487E91DEE79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -947,14 +1224,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="0e3eb1a6-496e-4caf-a79e-edeae59da28b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E242C474-6AB9-443D-B939-8B932E7DF18F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>